<commit_message>
thông tin đăng nhập
nguyen
</commit_message>
<xml_diff>
--- a/Thông tin đăng nhập.xlsx
+++ b/Thông tin đăng nhập.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KẾ HOẠCH\Yolo-Fashion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\Yolo-Fashion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF5625D-C449-4A12-A211-4434BA7343B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6288AF3-55FF-4248-8E4A-4221F800C3CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A794C49C-91FA-4CDB-9EBB-5ED38970F728}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="51">
   <si>
     <t>Tên TK</t>
   </si>
@@ -64,18 +64,12 @@
     <t>yolofashion@88</t>
   </si>
   <si>
-    <t>tiktok</t>
-  </si>
-  <si>
     <t>yolo.fashion88</t>
   </si>
   <si>
     <t>Yolofashion@88</t>
   </si>
   <si>
-    <t>CLONE TIKTOK</t>
-  </si>
-  <si>
     <t>lannhi</t>
   </si>
   <si>
@@ -148,16 +142,46 @@
     <t>sn: 5/5/2000</t>
   </si>
   <si>
-    <t>hacklike68</t>
-  </si>
-  <si>
-    <t>TÊN ĐN</t>
-  </si>
-  <si>
     <t>yolo88</t>
   </si>
   <si>
     <t>Yolo123@</t>
+  </si>
+  <si>
+    <t>Thanh Mai</t>
+  </si>
+  <si>
+    <t>thoitrang12345</t>
+  </si>
+  <si>
+    <t>thoitrang98701</t>
+  </si>
+  <si>
+    <t>sn:1/1//1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLONE </t>
+  </si>
+  <si>
+    <t>TIKTOK</t>
+  </si>
+  <si>
+    <t>FB</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>GMAIL</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Hacklive68</t>
+  </si>
+  <si>
+    <t>Tiktok</t>
   </si>
 </sst>
 </file>
@@ -238,7 +262,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -263,9 +287,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -581,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6ED7254-901C-4224-AA89-5DE9C65321E0}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -593,17 +620,18 @@
     <col min="2" max="2" width="32.26953125" customWidth="1"/>
     <col min="3" max="3" width="20.08984375" customWidth="1"/>
     <col min="4" max="4" width="43.6328125" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -617,7 +645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -631,7 +659,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -645,60 +673,66 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>38</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>14</v>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>0</v>
       </c>
@@ -711,148 +745,195 @@
       <c r="D13" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E13" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="E14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>10</v>
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+      <c r="E17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>28</v>
       </c>
-      <c r="C26" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="B19" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>32</v>
+      <c r="E19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B35" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C35" t="s">
-        <v>24</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>2</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>42</v>
+      <c r="C36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -866,17 +947,17 @@
     <hyperlink ref="C4" r:id="rId3" xr:uid="{2232FD74-5E77-4B41-99EE-D476FADFB5A1}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{84AEEB3E-29A8-4452-9430-1243F6B11140}"/>
     <hyperlink ref="B14" r:id="rId5" xr:uid="{5FFBD3C0-04A3-4121-8689-AED082BEDB9D}"/>
-    <hyperlink ref="B15" r:id="rId6" xr:uid="{AE345842-AC46-47F1-BA16-C0A86C11CBB3}"/>
-    <hyperlink ref="B16" r:id="rId7" xr:uid="{D716DBD7-59AA-40F7-A9F1-97F33C506D82}"/>
+    <hyperlink ref="B36" r:id="rId6" xr:uid="{AE345842-AC46-47F1-BA16-C0A86C11CBB3}"/>
+    <hyperlink ref="B37" r:id="rId7" xr:uid="{D716DBD7-59AA-40F7-A9F1-97F33C506D82}"/>
     <hyperlink ref="C14" r:id="rId8" xr:uid="{205B6CEF-8668-4470-AA83-43133E48149C}"/>
-    <hyperlink ref="B25" r:id="rId9" xr:uid="{3B6AA077-5FC3-4BAC-8CC2-8085F4BD8F29}"/>
-    <hyperlink ref="B26" r:id="rId10" xr:uid="{1AD26B79-B145-44F9-AD52-4399BE202813}"/>
-    <hyperlink ref="B27" r:id="rId11" xr:uid="{EBBBBC5D-CFEB-4B85-AA29-F526503A3155}"/>
-    <hyperlink ref="B17" r:id="rId12" xr:uid="{AD2152DC-162A-4B50-9B9C-40760C102E59}"/>
-    <hyperlink ref="C17" r:id="rId13" xr:uid="{451B5E22-C9B9-4F9B-B7E8-79087CDA914C}"/>
-    <hyperlink ref="B18" r:id="rId14" xr:uid="{22526125-C130-4364-A264-AACF6E8F080D}"/>
+    <hyperlink ref="B17" r:id="rId9" xr:uid="{3B6AA077-5FC3-4BAC-8CC2-8085F4BD8F29}"/>
+    <hyperlink ref="B18" r:id="rId10" xr:uid="{1AD26B79-B145-44F9-AD52-4399BE202813}"/>
+    <hyperlink ref="B19" r:id="rId11" xr:uid="{EBBBBC5D-CFEB-4B85-AA29-F526503A3155}"/>
+    <hyperlink ref="B15" r:id="rId12" xr:uid="{AD2152DC-162A-4B50-9B9C-40760C102E59}"/>
+    <hyperlink ref="C15" r:id="rId13" xr:uid="{451B5E22-C9B9-4F9B-B7E8-79087CDA914C}"/>
+    <hyperlink ref="B16" r:id="rId14" xr:uid="{22526125-C130-4364-A264-AACF6E8F080D}"/>
     <hyperlink ref="B35" r:id="rId15" xr:uid="{06E9FCD6-B18B-44EB-A2BF-6E1D160D9A00}"/>
-    <hyperlink ref="B42" r:id="rId16" xr:uid="{AA662370-6741-4678-B245-722DB8DF8959}"/>
+    <hyperlink ref="C10" r:id="rId16" xr:uid="{AA662370-6741-4678-B245-722DB8DF8959}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId17"/>

</xml_diff>